<commit_message>
Thêm nhóm roiter Công việc và các chức năng nhập dữ liệu, danh sách, thời gian
</commit_message>
<xml_diff>
--- a/data/72_nha.xlsx
+++ b/data/72_nha.xlsx
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Thêm file dữ liệu tra cứu 72_nha.xlsx
</commit_message>
<xml_diff>
--- a/data/72_nha.xlsx
+++ b/data/72_nha.xlsx
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cập nhật danh sách nhà từ Excel
</commit_message>
<xml_diff>
--- a/data/72_nha.xlsx
+++ b/data/72_nha.xlsx
@@ -756,38 +756,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.08203125" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.08203125" customWidth="1"/>
+    <col min="3" max="3" width="19.08203125" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" customWidth="1"/>
     <col min="5" max="5" width="16.08203125" customWidth="1"/>
     <col min="6" max="6" width="16.25" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="2"/>
-    <col min="13" max="13" width="31.1640625" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="2"/>
+    <col min="12" max="12" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
@@ -807,52 +807,52 @@
       <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
       <c r="M1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -872,34 +872,34 @@
       <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2">
+      <c r="K2" s="2">
         <v>8</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="M2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>